<commit_message>
modifs de sessions possible
</commit_message>
<xml_diff>
--- a/avancement.xlsx
+++ b/avancement.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elève\Documents\lycée\terminale\NSI\projets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\lycée\terminale\NSI\SchoolChoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D410D5BA-71AA-4A27-B917-0CE988B6B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592CF3A3-9D54-432A-B189-331280B5E199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B13041D5-606D-40CD-8394-3D43879D5851}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B13041D5-606D-40CD-8394-3D43879D5851}"/>
   </bookViews>
   <sheets>
     <sheet name="05 05 22" sheetId="1" r:id="rId1"/>
-    <sheet name="12 05 22" sheetId="2" r:id="rId2"/>
-    <sheet name="17 05 22" sheetId="3" r:id="rId3"/>
-    <sheet name="22 05 22" sheetId="4" r:id="rId4"/>
+    <sheet name="12 05 22" sheetId="5" r:id="rId2"/>
+    <sheet name="17 05 22" sheetId="7" r:id="rId3"/>
+    <sheet name="22 05 22" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
   <si>
     <t>Terminé </t>
   </si>
@@ -84,9 +82,6 @@
     <t>voir session </t>
   </si>
   <si>
-    <t>modifier session </t>
-  </si>
-  <si>
     <t>supprimer session </t>
   </si>
   <si>
@@ -106,13 +101,22 @@
   </si>
   <si>
     <t>envoyer résultats à la session</t>
+  </si>
+  <si>
+    <t>modifier nom session </t>
+  </si>
+  <si>
+    <t>ajouter élève à une session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer élève d'une session </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +169,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF9900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -241,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,12 +286,29 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF279D00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -590,16 +617,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C144C1D6-4756-4198-9FC6-C5EE2BEBECDF}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -656,52 +683,62 @@
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>15</v>
+      <c r="B6" s="15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="13" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -711,39 +748,397 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA80D74-05F4-42D2-9157-C020EA98853F}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6443E3F-B605-4B99-9DF1-F9D1310FB6E7}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B542B585-4BB6-4EA8-B0DB-A5FD221544B5}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8E4258-ABB2-4450-B988-7C52400ADE6C}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC262B-5CB1-4FA7-A555-D6D4786FCD2B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF88AE7C-A184-418E-89B1-C4A4C5343E6D}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fonction connexion à une session fonctionnelle
</commit_message>
<xml_diff>
--- a/avancement.xlsx
+++ b/avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\lycée\terminale\NSI\SchoolChoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592CF3A3-9D54-432A-B189-331280B5E199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C101BB94-4B99-4D8A-80B5-1A24F18E0FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B13041D5-606D-40CD-8394-3D43879D5851}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -752,7 +752,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +807,7 @@
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8E4258-ABB2-4450-B988-7C52400ADE6C}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +965,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -977,7 +977,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>